<commit_message>
moved Mettingprotocols to sub folder and added protocol from 2017-04-10
</commit_message>
<xml_diff>
--- a/documents/tests/Testprotokoll und Testbericht Vorlage.xlsx
+++ b/documents/tests/Testprotokoll und Testbericht Vorlage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Testprotokoll" sheetId="1" r:id="rId1"/>
@@ -421,28 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,16 +429,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,6 +492,9 @@
           <cell r="A10">
             <v>1</v>
           </cell>
+        </row>
+        <row r="400">
+          <cell r="A400"/>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -764,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -782,18 +785,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="3"/>
@@ -816,7 +819,7 @@
       </c>
       <c r="C6" s="10">
         <f ca="1">NOW()</f>
-        <v>42835.509452662038</v>
+        <v>42835.513700347219</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -858,7 +861,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="22">
         <v>1</v>
       </c>
       <c r="B11" s="15"/>
@@ -866,7 +869,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="23">
         <v>2</v>
       </c>
       <c r="B12" s="7"/>
@@ -874,229 +877,229 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="7"/>
       <c r="C14" s="14"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="7"/>
       <c r="C15" s="14"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="7"/>
       <c r="C16" s="14"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="7"/>
       <c r="C17" s="14"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="7"/>
       <c r="C18" s="14"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="7"/>
       <c r="C19" s="14"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="7"/>
       <c r="C20" s="14"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="7"/>
       <c r="C21" s="14"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="7"/>
       <c r="C22" s="14"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="7"/>
       <c r="C23" s="14"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="7"/>
       <c r="C24" s="14"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="7"/>
       <c r="C25" s="14"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="7"/>
       <c r="C26" s="14"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="7"/>
       <c r="C27" s="14"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="7"/>
       <c r="C28" s="14"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="7"/>
       <c r="C29" s="14"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="7"/>
       <c r="C30" s="14"/>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="7"/>
       <c r="C31" s="14"/>
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="7"/>
       <c r="C32" s="14"/>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="7"/>
       <c r="C33" s="14"/>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="7"/>
       <c r="C34" s="14"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="7"/>
       <c r="C35" s="14"/>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="7"/>
       <c r="C36" s="14"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="7"/>
       <c r="C37" s="14"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="7"/>
       <c r="C38" s="14"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="7"/>
       <c r="C39" s="14"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="7"/>
       <c r="C40" s="14"/>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="7"/>
       <c r="C41" s="14"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="7"/>
       <c r="C42" s="14"/>
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="7"/>
       <c r="C43" s="14"/>
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="7"/>
       <c r="C44" s="14"/>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="7"/>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="7"/>
       <c r="C46" s="14"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="7"/>
       <c r="C47" s="14"/>
       <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="7"/>
       <c r="C48" s="14"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="7"/>
       <c r="C49" s="14"/>
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="7"/>
       <c r="C50" s="14"/>
       <c r="D50" s="7"/>
@@ -1114,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -1130,20 +1133,20 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,73 +1155,73 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="7">
         <f>COUNTA([1]Tabelle1!$A$10:'[1]Tabelle1'!$A$400)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="21">
         <f>COUNTA(Testprotokoll!A11:'Testprotokoll'!A50)</f>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="21"/>
       <c r="E10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="21"/>
       <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="21"/>
       <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="31"/>
       <c r="D15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -1228,14 +1231,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="26"/>
+      <c r="E18" s="20"/>
       <c r="F18" t="s">
         <v>20</v>
       </c>
@@ -1251,11 +1254,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="28" t="s">
+      <c r="C21" s="29"/>
+      <c r="D21" s="21" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1270,11 +1273,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="28" t="s">
+      <c r="C24" s="29"/>
+      <c r="D24" s="21" t="s">
         <v>35</v>
       </c>
       <c r="F24" t="s">
@@ -1297,11 +1300,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="28" t="s">
+      <c r="C29" s="29"/>
+      <c r="D29" s="21" t="s">
         <v>40</v>
       </c>
       <c r="F29" t="s">
@@ -1325,10 +1328,10 @@
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -1357,6 +1360,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="A44:B44"/>
@@ -1364,11 +1372,6 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21 D18">

</xml_diff>

<commit_message>
added my first tests and test cases and merged the file with calvins test cases
</commit_message>
<xml_diff>
--- a/documents/tests/Testprotokoll und Testbericht Vorlage.xlsx
+++ b/documents/tests/Testprotokoll und Testbericht Vorlage.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Calvin 1/Dropbox/TU/4. Semester/SEPM/ue/proj_ss17_sepm_inso_07/documents/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\proj_ss17_sepm_inso_07\documents\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="13340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="12270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Testprotokoll" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,9 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -185,11 +179,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,15 +206,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,12 +217,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,11 +231,11 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -263,7 +244,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -271,22 +252,22 @@
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -295,74 +276,74 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -370,32 +351,32 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,11 +462,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,23 +764,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="6" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -811,7 +790,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
@@ -819,43 +798,43 @@
       <c r="E3" s="13"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="10">
         <f ca="1">NOW()</f>
-        <v>42877.557718402779</v>
+        <v>42877.950988194447</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="6"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="6"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="11"/>
@@ -864,7 +843,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>5</v>
       </c>
@@ -878,259 +857,245 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>1</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="35"/>
-    </row>
-    <row r="12" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>2</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="36"/>
-    </row>
-    <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22">
-        <v>3</v>
-      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
       <c r="B13" s="7"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="36"/>
-    </row>
-    <row r="14" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23">
-        <v>4</v>
-      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
       <c r="B14" s="7"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22">
-        <v>5</v>
-      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="7"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="36"/>
-    </row>
-    <row r="16" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23">
-        <v>6</v>
-      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="7"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22">
-        <v>7</v>
-      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
       <c r="B17" s="7"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23">
-        <v>8</v>
-      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
       <c r="B18" s="7"/>
       <c r="C18" s="14"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22">
-        <v>9</v>
-      </c>
+    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
       <c r="B19" s="7"/>
       <c r="C19" s="14"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="7"/>
       <c r="C20" s="14"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="7"/>
       <c r="C21" s="14"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="7"/>
       <c r="C22" s="14"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="7"/>
       <c r="C23" s="14"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="7"/>
       <c r="C24" s="14"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="7"/>
       <c r="C25" s="14"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="7"/>
       <c r="C26" s="14"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="7"/>
       <c r="C27" s="14"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="7"/>
       <c r="C28" s="14"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="7"/>
       <c r="C29" s="14"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="7"/>
       <c r="C30" s="14"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="7"/>
       <c r="C31" s="14"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="7"/>
       <c r="C32" s="14"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="7"/>
       <c r="C33" s="14"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="7"/>
       <c r="C34" s="14"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="7"/>
       <c r="C35" s="14"/>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="7"/>
       <c r="C36" s="14"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="7"/>
       <c r="C37" s="14"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="7"/>
       <c r="C38" s="14"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="7"/>
       <c r="C39" s="14"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="7"/>
       <c r="C40" s="14"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="7"/>
       <c r="C41" s="14"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="7"/>
       <c r="C42" s="14"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="7"/>
       <c r="C43" s="14"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="7"/>
       <c r="C44" s="14"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="B45" s="7"/>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="7"/>
       <c r="C46" s="14"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="7"/>
       <c r="C47" s="14"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="7"/>
       <c r="C48" s="14"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="7"/>
       <c r="C49" s="14"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="7"/>
       <c r="C50" s="14"/>
@@ -1149,21 +1114,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.6640625" customWidth="1"/>
+    <col min="1" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -1173,7 +1138,7 @@
       <c r="E2" s="26"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="27"/>
       <c r="C3" s="30"/>
@@ -1181,12 +1146,12 @@
       <c r="E3" s="28"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
@@ -1194,10 +1159,10 @@
       <c r="C8" s="31"/>
       <c r="D8" s="7">
         <f>COUNTA([1]Tabelle1!$A$10:'[1]Tabelle1'!$A$400)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>14</v>
       </c>
@@ -1205,10 +1170,10 @@
       <c r="C9" s="31"/>
       <c r="D9" s="21">
         <f>COUNTA(Testprotokoll!A11:'Testprotokoll'!A50)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
@@ -1230,7 +1195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>13</v>
       </c>
@@ -1241,8 +1206,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>19</v>
       </c>
@@ -1251,18 +1216,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="24"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="E17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="32" t="s">
         <v>23</v>
       </c>
@@ -1275,17 +1240,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
         <v>25</v>
       </c>
@@ -1294,17 +1259,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="32" t="s">
         <v>34</v>
       </c>
@@ -1316,22 +1281,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="32" t="s">
         <v>33</v>
       </c>
@@ -1343,49 +1308,49 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="34"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>47</v>
       </c>

</xml_diff>